<commit_message>
updates - data QAQC
</commit_message>
<xml_diff>
--- a/Data Files/PerkinsusMD&VA2.xlsx
+++ b/Data Files/PerkinsusMD&VA2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariahkachmar/Documents/UMBC/GitHub/Meta-analysis-Perkinsus-Marinus/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A100D4-9CE7-BD41-BC09-3BBABF4AA0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628B5525-BB5B-E248-AE4B-7D6AFCC9477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2211" workbookViewId="0">
-      <selection activeCell="D2241" sqref="D2241"/>
+    <sheetView tabSelected="1" topLeftCell="A617" workbookViewId="0">
+      <selection activeCell="K634" sqref="K634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21735,7 +21735,7 @@
         <v>94</v>
       </c>
       <c r="J639">
-        <v>54</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>